<commit_message>
Fixed memory leaks with virtual destructor
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\banner.main.ad.rit.edu\students\aa6096\IGMProfile\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\banner.main.ad.rit.edu\students\jas2715\IGMProfile\Desktop\GitHub\CatBowling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>IGME 309 Final Project Fall 2013 Grading Guide</t>
   </si>
@@ -33,12 +33,6 @@
   </si>
   <si>
     <t>Total Grade</t>
-  </si>
-  <si>
-    <t>&lt;Student 1&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Student 2&gt;</t>
   </si>
   <si>
     <t>Criteria</t>
@@ -256,6 +250,15 @@
   </si>
   <si>
     <t>Implement a custom GUI system.</t>
+  </si>
+  <si>
+    <t>CatBowling\include\Visual Leak Detector</t>
+  </si>
+  <si>
+    <t>Rebecca Vessal</t>
+  </si>
+  <si>
+    <t>Jennifer Stanton</t>
   </si>
 </sst>
 </file>
@@ -772,6 +775,123 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -804,123 +924,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1206,7 +1209,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,92 +1793,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="31" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34">
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73">
         <f>((F70/E70)*100)</f>
         <v>0</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="32" t="s">
+      <c r="A3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="A5" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41"/>
+      <c r="A6" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="6">
         <v>10</v>
       </c>
@@ -1884,12 +1887,12 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="44"/>
+      <c r="A7" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="8">
         <f>SUM(E6:E6)</f>
         <v>10</v>
@@ -1902,24 +1905,24 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="A8" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
+      <c r="A9" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="12">
         <v>10</v>
       </c>
@@ -1928,12 +1931,12 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50"/>
+      <c r="A10" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="12">
         <v>10</v>
       </c>
@@ -1942,12 +1945,12 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
+      <c r="A11" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="12">
         <v>10</v>
       </c>
@@ -1956,12 +1959,12 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41"/>
+      <c r="A12" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="12">
         <v>10</v>
       </c>
@@ -1970,12 +1973,12 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44"/>
+      <c r="A13" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="46"/>
       <c r="E13" s="8">
         <f>SUM(E9:E12)</f>
         <v>40</v>
@@ -1988,24 +1991,24 @@
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="A14" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="41"/>
+      <c r="A15" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="12">
         <v>10</v>
       </c>
@@ -2014,12 +2017,12 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41"/>
+      <c r="A16" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="12">
         <v>10</v>
       </c>
@@ -2028,12 +2031,12 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
+      <c r="A17" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="12">
         <v>40</v>
       </c>
@@ -2042,12 +2045,12 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
+      <c r="A18" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="8">
         <f>SUM(E15:E17)</f>
         <v>60</v>
@@ -2060,24 +2063,24 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
+      <c r="A19" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
+      <c r="A20" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="12">
         <v>5</v>
       </c>
@@ -2086,12 +2089,12 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="41"/>
+      <c r="A21" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="12">
         <v>5</v>
       </c>
@@ -2100,12 +2103,12 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="41"/>
+      <c r="A22" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="12">
         <v>20</v>
       </c>
@@ -2114,12 +2117,12 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
+      <c r="A23" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46"/>
       <c r="E23" s="8">
         <f>SUM(E20:E22)</f>
         <v>30</v>
@@ -2132,305 +2135,307 @@
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:9" ht="29.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
+      <c r="A24" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
+      <c r="A25" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="41"/>
+      <c r="A26" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="37"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="41"/>
+      <c r="A27" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
+      <c r="A28" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
     </row>
     <row r="29" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="41"/>
+      <c r="A29" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="41"/>
+      <c r="A30" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="41"/>
+      <c r="A31" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="41"/>
+      <c r="A32" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="37"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="41"/>
+      <c r="A33" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
+      <c r="A34" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="41"/>
+      <c r="A35" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="37"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="41"/>
+      <c r="A36" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="37"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="41"/>
+      <c r="A37" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="41"/>
+      <c r="A38" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="41"/>
+      <c r="A39" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="41"/>
+      <c r="A40" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="37"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
-      <c r="G40" s="13"/>
+      <c r="G40" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="41"/>
+      <c r="A41" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
+      <c r="A42" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
     </row>
     <row r="43" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="41"/>
+      <c r="A43" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="37"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="41"/>
+      <c r="A44" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="37"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="41"/>
+      <c r="A45" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="13"/>
       <c r="H45" s="21"/>
     </row>
     <row r="46" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="66"/>
+      <c r="A46" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="26"/>
       <c r="H46" s="22"/>
       <c r="I46" s="2"/>
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="B47" s="40"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="41"/>
+      <c r="A47" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="37"/>
       <c r="E47" s="12"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="68"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="28"/>
       <c r="H47" s="22"/>
       <c r="I47" s="2"/>
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" s="62"/>
-      <c r="C48" s="62"/>
-      <c r="D48" s="63"/>
+      <c r="A48" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="49"/>
       <c r="E48" s="14">
         <f>SUM(E26:E47)</f>
         <v>0</v>
@@ -2443,25 +2448,25 @@
       <c r="H48" s="23"/>
     </row>
     <row r="49" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49" s="46"/>
-      <c r="C49" s="46"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="54"/>
+      <c r="A49" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="54"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="56"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B50" s="40"/>
-      <c r="C50" s="40"/>
-      <c r="D50" s="41"/>
+      <c r="A50" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="37"/>
       <c r="E50" s="12">
         <v>5</v>
       </c>
@@ -2470,12 +2475,12 @@
       <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="41"/>
+      <c r="A51" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="37"/>
       <c r="E51" s="12">
         <v>5</v>
       </c>
@@ -2484,12 +2489,12 @@
       <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="40"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="41"/>
+      <c r="A52" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="37"/>
       <c r="E52" s="12">
         <v>5</v>
       </c>
@@ -2498,12 +2503,12 @@
       <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="41"/>
+      <c r="A53" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="37"/>
       <c r="E53" s="12">
         <v>10</v>
       </c>
@@ -2512,12 +2517,12 @@
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B54" s="40"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="41"/>
+      <c r="A54" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="37"/>
       <c r="E54" s="12">
         <v>50</v>
       </c>
@@ -2526,12 +2531,12 @@
       <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55" s="40"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="41"/>
+      <c r="A55" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="37"/>
       <c r="E55" s="12">
         <v>10</v>
       </c>
@@ -2540,12 +2545,12 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B56" s="40"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="41"/>
+      <c r="A56" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="37"/>
       <c r="E56" s="12">
         <v>10</v>
       </c>
@@ -2554,12 +2559,12 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="41"/>
+      <c r="A57" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="37"/>
       <c r="E57" s="12">
         <v>20</v>
       </c>
@@ -2568,12 +2573,12 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="41"/>
+      <c r="A58" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="37"/>
       <c r="E58" s="12">
         <v>20</v>
       </c>
@@ -2582,12 +2587,12 @@
       <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="B59" s="40"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="41"/>
+      <c r="A59" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="37"/>
       <c r="E59" s="12">
         <v>20</v>
       </c>
@@ -2596,12 +2601,12 @@
       <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="41"/>
+      <c r="A60" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="37"/>
       <c r="E60" s="12">
         <v>30</v>
       </c>
@@ -2610,12 +2615,12 @@
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="40"/>
-      <c r="C61" s="40"/>
-      <c r="D61" s="41"/>
+      <c r="A61" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="12">
         <v>10</v>
       </c>
@@ -2624,12 +2629,12 @@
       <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62" s="40"/>
-      <c r="C62" s="40"/>
-      <c r="D62" s="41"/>
+      <c r="A62" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="12">
         <v>20</v>
       </c>
@@ -2638,12 +2643,12 @@
       <c r="H62" s="13"/>
     </row>
     <row r="63" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63" s="40"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="41"/>
+      <c r="A63" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="37"/>
       <c r="E63" s="12">
         <v>30</v>
       </c>
@@ -2652,12 +2657,12 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="B64" s="40"/>
-      <c r="C64" s="40"/>
-      <c r="D64" s="41"/>
+      <c r="A64" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="37"/>
       <c r="E64" s="12">
         <v>20</v>
       </c>
@@ -2666,12 +2671,12 @@
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="40"/>
-      <c r="C65" s="40"/>
-      <c r="D65" s="41"/>
+      <c r="A65" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="37"/>
       <c r="E65" s="12">
         <v>20</v>
       </c>
@@ -2680,12 +2685,12 @@
       <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B66" s="40"/>
-      <c r="C66" s="40"/>
-      <c r="D66" s="41"/>
+      <c r="A66" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="37"/>
       <c r="E66" s="12">
         <v>20</v>
       </c>
@@ -2694,12 +2699,12 @@
       <c r="H66" s="13"/>
     </row>
     <row r="67" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B67" s="40"/>
-      <c r="C67" s="40"/>
-      <c r="D67" s="41"/>
+      <c r="A67" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="37"/>
       <c r="E67" s="12">
         <v>20</v>
       </c>
@@ -2708,31 +2713,31 @@
       <c r="H67" s="13"/>
     </row>
     <row r="68" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="B68" s="40"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="41"/>
-      <c r="E68" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="F68" s="69"/>
+      <c r="A68" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F68" s="29"/>
       <c r="G68" s="22"/>
       <c r="H68" s="22"/>
     </row>
     <row r="69" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="B69" s="43"/>
-      <c r="C69" s="43"/>
-      <c r="D69" s="44"/>
-      <c r="E69" s="73">
+      <c r="A69" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69" s="45"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="46"/>
+      <c r="E69" s="33">
         <f>SUM(E50:E67)</f>
         <v>325</v>
       </c>
-      <c r="F69" s="72">
+      <c r="F69" s="32">
         <f>SUM(F50:F68)</f>
         <v>0</v>
       </c>
@@ -2740,17 +2745,17 @@
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="58" t="s">
-        <v>36</v>
-      </c>
-      <c r="B70" s="59"/>
-      <c r="C70" s="59"/>
-      <c r="D70" s="60"/>
-      <c r="E70" s="70">
+      <c r="A70" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="43"/>
+      <c r="E70" s="30">
         <f>SUM(E7,E13,E18,E23)</f>
         <v>140</v>
       </c>
-      <c r="F70" s="71">
+      <c r="F70" s="31">
         <f>MAX(0,SUM(F7,F13,F18,F23,F48,F69))</f>
         <v>0</v>
       </c>
@@ -3332,6 +3337,72 @@
     <row r="153" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A61:D61"/>
     <mergeCell ref="E25:H25"/>
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="E34:H34"/>
@@ -3348,72 +3419,6 @@
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Conservation of linear momentum implemented. Collision response fixed.
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
   <si>
     <t>IGME 309 Final Project Fall 2013 Grading Guide</t>
   </si>
@@ -259,6 +259,24 @@
   </si>
   <si>
     <t>Jennifer Stanton</t>
+  </si>
+  <si>
+    <t>Octree.h</t>
+  </si>
+  <si>
+    <t>Polyhedron.h-&gt;PhysicsComponent</t>
+  </si>
+  <si>
+    <t>Polyhedron-&gt;eulerIntegrationUpdate();</t>
+  </si>
+  <si>
+    <t>glm used for math instead of Angel</t>
+  </si>
+  <si>
+    <t>Polyhedron-&gt;testCollision();</t>
+  </si>
+  <si>
+    <t>Keyboard: space, p, r, q or esc</t>
   </si>
 </sst>
 </file>
@@ -805,6 +823,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -817,24 +877,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -844,14 +886,23 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -860,70 +911,37 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1209,7 +1227,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,58 +1811,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="70" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="71" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73">
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44">
         <f>((F70/E70)*100)</f>
         <v>0</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="71" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1860,25 +1878,25 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="6">
         <v>10</v>
       </c>
@@ -1887,12 +1905,12 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="8">
         <f>SUM(E6:E6)</f>
         <v>10</v>
@@ -1905,80 +1923,88 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="12">
         <v>10</v>
       </c>
       <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="12">
         <v>10</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="13" t="s">
+        <v>82</v>
+      </c>
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="12">
         <v>10</v>
       </c>
       <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
+      <c r="G11" s="13" t="s">
+        <v>80</v>
+      </c>
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="12">
         <v>10</v>
       </c>
       <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
+      <c r="G12" s="13" t="s">
+        <v>82</v>
+      </c>
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="8">
         <f>SUM(E9:E12)</f>
         <v>40</v>
@@ -1991,24 +2017,24 @@
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="37"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="12">
         <v>10</v>
       </c>
@@ -2017,12 +2043,12 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="37"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="12">
         <v>10</v>
       </c>
@@ -2031,26 +2057,28 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="12">
         <v>40</v>
       </c>
       <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="46"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="8">
         <f>SUM(E15:E17)</f>
         <v>60</v>
@@ -2063,24 +2091,24 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
     </row>
     <row r="20" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="12">
         <v>5</v>
       </c>
@@ -2089,12 +2117,12 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="12">
         <v>5</v>
       </c>
@@ -2103,12 +2131,12 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="51"/>
       <c r="E22" s="12">
         <v>20</v>
       </c>
@@ -2117,12 +2145,12 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="46"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="8">
         <f>SUM(E20:E22)</f>
         <v>30</v>
@@ -2135,205 +2163,207 @@
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:9" ht="29.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
     </row>
     <row r="26" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
     </row>
     <row r="29" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="37"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="37"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="51"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="37"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
-      <c r="G31" s="13"/>
+      <c r="G31" s="13" t="s">
+        <v>83</v>
+      </c>
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="51"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="37"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="51"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
     </row>
     <row r="35" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="51"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="37"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="51"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="37"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="51"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="51"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="51"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="37"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="51"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="13" t="s">
@@ -2342,72 +2372,72 @@
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="37"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="51"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
     </row>
     <row r="43" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="37"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="51"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="37"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="51"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="37"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="51"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="13"/>
       <c r="H45" s="21"/>
     </row>
     <row r="46" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="37"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="51"/>
       <c r="E46" s="24"/>
       <c r="F46" s="25"/>
       <c r="G46" s="26"/>
@@ -2416,12 +2446,12 @@
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="37"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="51"/>
       <c r="E47" s="12"/>
       <c r="F47" s="27"/>
       <c r="G47" s="28"/>
@@ -2430,12 +2460,12 @@
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="47" t="s">
+      <c r="A48" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="49"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="70"/>
       <c r="E48" s="14">
         <f>SUM(E26:E47)</f>
         <v>0</v>
@@ -2448,25 +2478,25 @@
       <c r="H48" s="23"/>
     </row>
     <row r="49" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="53" t="s">
+      <c r="A49" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="54"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="56"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="64"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="37"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="51"/>
       <c r="E50" s="12">
         <v>5</v>
       </c>
@@ -2475,12 +2505,12 @@
       <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="37"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="51"/>
       <c r="E51" s="12">
         <v>5</v>
       </c>
@@ -2489,12 +2519,12 @@
       <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="37"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="51"/>
       <c r="E52" s="12">
         <v>5</v>
       </c>
@@ -2503,12 +2533,12 @@
       <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="37"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="51"/>
       <c r="E53" s="12">
         <v>10</v>
       </c>
@@ -2517,12 +2547,12 @@
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="35" t="s">
+      <c r="A54" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="37"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="51"/>
       <c r="E54" s="12">
         <v>50</v>
       </c>
@@ -2531,12 +2561,12 @@
       <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="37"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="51"/>
       <c r="E55" s="12">
         <v>10</v>
       </c>
@@ -2545,12 +2575,12 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="37"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="51"/>
       <c r="E56" s="12">
         <v>10</v>
       </c>
@@ -2559,12 +2589,12 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="37"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="51"/>
       <c r="E57" s="12">
         <v>20</v>
       </c>
@@ -2573,12 +2603,12 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="37"/>
+      <c r="B58" s="50"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="51"/>
       <c r="E58" s="12">
         <v>20</v>
       </c>
@@ -2587,12 +2617,12 @@
       <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="35" t="s">
+      <c r="A59" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="37"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="51"/>
       <c r="E59" s="12">
         <v>20</v>
       </c>
@@ -2601,12 +2631,12 @@
       <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="37"/>
+      <c r="B60" s="50"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="51"/>
       <c r="E60" s="12">
         <v>30</v>
       </c>
@@ -2615,12 +2645,12 @@
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="37"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="51"/>
       <c r="E61" s="12">
         <v>10</v>
       </c>
@@ -2629,12 +2659,12 @@
       <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="35" t="s">
+      <c r="A62" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="37"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="51"/>
       <c r="E62" s="12">
         <v>20</v>
       </c>
@@ -2643,12 +2673,12 @@
       <c r="H62" s="13"/>
     </row>
     <row r="63" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="37"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="51"/>
       <c r="E63" s="12">
         <v>30</v>
       </c>
@@ -2657,12 +2687,12 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="37"/>
+      <c r="B64" s="50"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="51"/>
       <c r="E64" s="12">
         <v>20</v>
       </c>
@@ -2671,12 +2701,12 @@
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="35" t="s">
+      <c r="A65" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="37"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="51"/>
       <c r="E65" s="12">
         <v>20</v>
       </c>
@@ -2685,12 +2715,12 @@
       <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="37"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="51"/>
       <c r="E66" s="12">
         <v>20</v>
       </c>
@@ -2699,12 +2729,12 @@
       <c r="H66" s="13"/>
     </row>
     <row r="67" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="37"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="51"/>
       <c r="E67" s="12">
         <v>20</v>
       </c>
@@ -2713,26 +2743,28 @@
       <c r="H67" s="13"/>
     </row>
     <row r="68" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="35" t="s">
+      <c r="A68" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="37"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="51"/>
       <c r="E68" s="24" t="s">
         <v>25</v>
       </c>
       <c r="F68" s="29"/>
-      <c r="G68" s="22"/>
+      <c r="G68" s="22" t="s">
+        <v>81</v>
+      </c>
       <c r="H68" s="22"/>
     </row>
     <row r="69" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="44" t="s">
+      <c r="A69" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="46"/>
+      <c r="B69" s="53"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="54"/>
       <c r="E69" s="33">
         <f>SUM(E50:E67)</f>
         <v>325</v>
@@ -2745,12 +2777,12 @@
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B70" s="42"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="43"/>
+      <c r="B70" s="72"/>
+      <c r="C70" s="72"/>
+      <c r="D70" s="73"/>
       <c r="E70" s="30">
         <f>SUM(E7,E13,E18,E23)</f>
         <v>140</v>
@@ -3337,35 +3369,43 @@
     <row r="153" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A48:D48"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="E24:H24"/>
     <mergeCell ref="A64:D64"/>
@@ -3382,43 +3422,35 @@
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="A55:D55"/>
     <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed merge conflict and updated grading sheet
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\banner.main.ad.rit.edu\students\jas2715\IGMProfile\Desktop\GitHub\CatBowling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\banner.main.ad.rit.edu\students\rbv7405\IGMProfile\Desktop\GitHub\CatBowling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <t>IGME 309 Final Project Fall 2013 Grading Guide</t>
   </si>
@@ -270,13 +270,37 @@
     <t>Polyhedron-&gt;eulerIntegrationUpdate();</t>
   </si>
   <si>
-    <t>glm used for math instead of Angel</t>
-  </si>
-  <si>
     <t>Polyhedron-&gt;testCollision();</t>
   </si>
   <si>
     <t>Keyboard: space, p, r, q or esc</t>
+  </si>
+  <si>
+    <t>BezierSurfaceController.h</t>
+  </si>
+  <si>
+    <t>Using VBOs and VAOS in Polyhedron.h, BezierCurve.h, BezierSurface.h.  Fragment and vertex shaders can be found at these files: fshader.glsl and vshader.glsl</t>
+  </si>
+  <si>
+    <t>Color changing of polyhedrons in fragment shader</t>
+  </si>
+  <si>
+    <t>All files in project have headers and cpp</t>
+  </si>
+  <si>
+    <t>All files in project have include guards</t>
+  </si>
+  <si>
+    <t>Comments above parts of code taken from other sources can be found in various files in the project</t>
+  </si>
+  <si>
+    <t>glm used for math instead of Angel, dynamic fragment colors for polyhedrons</t>
+  </si>
+  <si>
+    <t>Inheritance is used with specialized polyhedrons</t>
+  </si>
+  <si>
+    <t>See all files in project</t>
   </si>
 </sst>
 </file>
@@ -823,6 +847,93 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -855,93 +966,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1227,7 +1251,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,58 +1835,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="41" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="42" t="s">
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44">
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73">
         <f>((F70/E70)*100)</f>
         <v>0</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="42" t="s">
+      <c r="A3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="73"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="65"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1878,25 +1902,25 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="6">
         <v>10</v>
       </c>
@@ -1905,12 +1929,12 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="54"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="8">
         <f>SUM(E6:E6)</f>
         <v>10</v>
@@ -1923,24 +1947,24 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="12">
         <v>10</v>
       </c>
@@ -1951,28 +1975,28 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="12">
         <v>10</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="12">
         <v>10</v>
       </c>
@@ -1983,28 +2007,28 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="51"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="12">
         <v>10</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="46"/>
       <c r="E13" s="8">
         <f>SUM(E9:E12)</f>
         <v>40</v>
@@ -2017,24 +2041,24 @@
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="12">
         <v>10</v>
       </c>
@@ -2043,12 +2067,12 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="12">
         <v>10</v>
       </c>
@@ -2057,12 +2081,12 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="12">
         <v>40</v>
       </c>
@@ -2073,12 +2097,12 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="8">
         <f>SUM(E15:E17)</f>
         <v>60</v>
@@ -2091,24 +2115,24 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="12">
         <v>5</v>
       </c>
@@ -2117,12 +2141,12 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="12">
         <v>5</v>
       </c>
@@ -2131,26 +2155,28 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="12">
         <v>20</v>
       </c>
       <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
+      <c r="G22" s="13" t="s">
+        <v>83</v>
+      </c>
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="54"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46"/>
       <c r="E23" s="8">
         <f>SUM(E20:E22)</f>
         <v>30</v>
@@ -2163,207 +2189,219 @@
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:9" ht="29.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="65" t="s">
+      <c r="A25" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="51"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="37"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
+      <c r="G26" s="13" t="s">
+        <v>84</v>
+      </c>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="51"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
+      <c r="G27" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
     </row>
     <row r="29" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="51"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="51"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="51"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="51"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="37"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="51"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="51"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="37"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
-      <c r="G35" s="13"/>
+      <c r="G35" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="51"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="37"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="51"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
-      <c r="G37" s="13"/>
+      <c r="G37" s="13" t="s">
+        <v>90</v>
+      </c>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="51"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
-      <c r="G38" s="13"/>
+      <c r="G38" s="13" t="s">
+        <v>86</v>
+      </c>
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="51"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
-      <c r="G39" s="13"/>
+      <c r="G39" s="13" t="s">
+        <v>87</v>
+      </c>
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="50"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="51"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="37"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="13" t="s">
@@ -2372,72 +2410,74 @@
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="51"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
-      <c r="G41" s="13"/>
+      <c r="G41" s="13" t="s">
+        <v>88</v>
+      </c>
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="65" t="s">
+      <c r="A42" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="66"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
     </row>
     <row r="43" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="51"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="37"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="49" t="s">
+      <c r="A44" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="51"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="37"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="51"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="13"/>
       <c r="H45" s="21"/>
     </row>
     <row r="46" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="s">
+      <c r="A46" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="51"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="37"/>
       <c r="E46" s="24"/>
       <c r="F46" s="25"/>
       <c r="G46" s="26"/>
@@ -2446,12 +2486,12 @@
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="51"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="37"/>
       <c r="E47" s="12"/>
       <c r="F47" s="27"/>
       <c r="G47" s="28"/>
@@ -2460,12 +2500,12 @@
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="68" t="s">
+      <c r="A48" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="69"/>
-      <c r="C48" s="69"/>
-      <c r="D48" s="70"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="49"/>
       <c r="E48" s="14">
         <f>SUM(E26:E47)</f>
         <v>0</v>
@@ -2478,25 +2518,25 @@
       <c r="H48" s="23"/>
     </row>
     <row r="49" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="55" t="s">
+      <c r="A49" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="56"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="64"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="56"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="49" t="s">
+      <c r="A50" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="50"/>
-      <c r="C50" s="50"/>
-      <c r="D50" s="51"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="37"/>
       <c r="E50" s="12">
         <v>5</v>
       </c>
@@ -2505,12 +2545,12 @@
       <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="51"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="37"/>
       <c r="E51" s="12">
         <v>5</v>
       </c>
@@ -2519,12 +2559,12 @@
       <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="51"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="37"/>
       <c r="E52" s="12">
         <v>5</v>
       </c>
@@ -2533,12 +2573,12 @@
       <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="49" t="s">
+      <c r="A53" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="50"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="51"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="37"/>
       <c r="E53" s="12">
         <v>10</v>
       </c>
@@ -2547,12 +2587,12 @@
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="49" t="s">
+      <c r="A54" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="50"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="51"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="37"/>
       <c r="E54" s="12">
         <v>50</v>
       </c>
@@ -2561,12 +2601,12 @@
       <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="49" t="s">
+      <c r="A55" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="51"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="37"/>
       <c r="E55" s="12">
         <v>10</v>
       </c>
@@ -2575,12 +2615,12 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="50"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="51"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="37"/>
       <c r="E56" s="12">
         <v>10</v>
       </c>
@@ -2589,12 +2629,12 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="49" t="s">
+      <c r="A57" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="51"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="37"/>
       <c r="E57" s="12">
         <v>20</v>
       </c>
@@ -2603,12 +2643,12 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="49" t="s">
+      <c r="A58" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="50"/>
-      <c r="C58" s="50"/>
-      <c r="D58" s="51"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="37"/>
       <c r="E58" s="12">
         <v>20</v>
       </c>
@@ -2617,12 +2657,12 @@
       <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="49" t="s">
+      <c r="A59" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="51"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="37"/>
       <c r="E59" s="12">
         <v>20</v>
       </c>
@@ -2631,12 +2671,12 @@
       <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="49" t="s">
+      <c r="A60" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="50"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="51"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="37"/>
       <c r="E60" s="12">
         <v>30</v>
       </c>
@@ -2645,12 +2685,12 @@
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="49" t="s">
+      <c r="A61" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="50"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="51"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="12">
         <v>10</v>
       </c>
@@ -2659,12 +2699,12 @@
       <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="49" t="s">
+      <c r="A62" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="50"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="51"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="12">
         <v>20</v>
       </c>
@@ -2673,12 +2713,12 @@
       <c r="H62" s="13"/>
     </row>
     <row r="63" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="49" t="s">
+      <c r="A63" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="50"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="51"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="37"/>
       <c r="E63" s="12">
         <v>30</v>
       </c>
@@ -2687,12 +2727,12 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="49" t="s">
+      <c r="A64" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="50"/>
-      <c r="C64" s="50"/>
-      <c r="D64" s="51"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="37"/>
       <c r="E64" s="12">
         <v>20</v>
       </c>
@@ -2701,12 +2741,12 @@
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="49" t="s">
+      <c r="A65" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="50"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="51"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="37"/>
       <c r="E65" s="12">
         <v>20</v>
       </c>
@@ -2715,12 +2755,12 @@
       <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="49" t="s">
+      <c r="A66" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="50"/>
-      <c r="C66" s="50"/>
-      <c r="D66" s="51"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="37"/>
       <c r="E66" s="12">
         <v>20</v>
       </c>
@@ -2729,12 +2769,12 @@
       <c r="H66" s="13"/>
     </row>
     <row r="67" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="49" t="s">
+      <c r="A67" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="50"/>
-      <c r="C67" s="50"/>
-      <c r="D67" s="51"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="37"/>
       <c r="E67" s="12">
         <v>20</v>
       </c>
@@ -2743,28 +2783,28 @@
       <c r="H67" s="13"/>
     </row>
     <row r="68" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="49" t="s">
+      <c r="A68" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="50"/>
-      <c r="C68" s="50"/>
-      <c r="D68" s="51"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="37"/>
       <c r="E68" s="24" t="s">
         <v>25</v>
       </c>
       <c r="F68" s="29"/>
       <c r="G68" s="22" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="H68" s="22"/>
     </row>
     <row r="69" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="52" t="s">
+      <c r="A69" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="53"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="54"/>
+      <c r="B69" s="45"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="46"/>
       <c r="E69" s="33">
         <f>SUM(E50:E67)</f>
         <v>325</v>
@@ -2777,12 +2817,12 @@
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="71" t="s">
+      <c r="A70" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B70" s="72"/>
-      <c r="C70" s="72"/>
-      <c r="D70" s="73"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="43"/>
       <c r="E70" s="30">
         <f>SUM(E7,E13,E18,E23)</f>
         <v>140</v>
@@ -3369,6 +3409,72 @@
     <row r="153" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A61:D61"/>
     <mergeCell ref="E25:H25"/>
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="E34:H34"/>
@@ -3385,72 +3491,6 @@
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Point to line collision. Game points implemented.
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
   <si>
     <t>IGME 309 Final Project Fall 2013 Grading Guide</t>
   </si>
@@ -277,6 +277,15 @@
   </si>
   <si>
     <t>Keyboard: space, p, r, q or esc</t>
+  </si>
+  <si>
+    <t>Line-&gt;checkAABB() // line to AABB</t>
+  </si>
+  <si>
+    <t>Console window</t>
+  </si>
+  <si>
+    <t>all header files</t>
   </si>
 </sst>
 </file>
@@ -823,6 +832,93 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -855,93 +951,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1226,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,58 +1820,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="41" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="42" t="s">
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44">
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73">
         <f>((F70/E70)*100)</f>
         <v>0</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="42" t="s">
+      <c r="A3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="73"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="65"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1878,25 +1887,25 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="6">
         <v>10</v>
       </c>
@@ -1905,12 +1914,12 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="54"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="8">
         <f>SUM(E6:E6)</f>
         <v>10</v>
@@ -1923,24 +1932,24 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="12">
         <v>10</v>
       </c>
@@ -1951,12 +1960,12 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="12">
         <v>10</v>
       </c>
@@ -1967,12 +1976,12 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="12">
         <v>10</v>
       </c>
@@ -1983,12 +1992,12 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="51"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="12">
         <v>10</v>
       </c>
@@ -1999,12 +2008,12 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="46"/>
       <c r="E13" s="8">
         <f>SUM(E9:E12)</f>
         <v>40</v>
@@ -2017,38 +2026,40 @@
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="12">
         <v>10</v>
       </c>
       <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="13" t="s">
+        <v>84</v>
+      </c>
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="12">
         <v>10</v>
       </c>
@@ -2057,12 +2068,12 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="12">
         <v>40</v>
       </c>
@@ -2073,12 +2084,12 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="8">
         <f>SUM(E15:E17)</f>
         <v>60</v>
@@ -2091,24 +2102,24 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="12">
         <v>5</v>
       </c>
@@ -2117,12 +2128,12 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="12">
         <v>5</v>
       </c>
@@ -2131,12 +2142,12 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="12">
         <v>20</v>
       </c>
@@ -2145,12 +2156,12 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="54"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46"/>
       <c r="E23" s="8">
         <f>SUM(E20:E22)</f>
         <v>30</v>
@@ -2163,97 +2174,99 @@
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:9" ht="29.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="65" t="s">
+      <c r="A25" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="51"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="37"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="51"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
     </row>
     <row r="29" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="51"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="51"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
-      <c r="G30" s="13"/>
+      <c r="G30" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="51"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="13" t="s">
@@ -2262,108 +2275,110 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="51"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="37"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="51"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="51"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="37"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="51"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="37"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="51"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="51"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="51"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
-      <c r="G39" s="13"/>
+      <c r="G39" s="13" t="s">
+        <v>86</v>
+      </c>
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="50"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="51"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="37"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="13" t="s">
@@ -2372,72 +2387,72 @@
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="51"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="65" t="s">
+      <c r="A42" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="66"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
     </row>
     <row r="43" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="51"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="37"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="49" t="s">
+      <c r="A44" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="51"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="37"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="51"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="13"/>
       <c r="H45" s="21"/>
     </row>
     <row r="46" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="s">
+      <c r="A46" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="51"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="37"/>
       <c r="E46" s="24"/>
       <c r="F46" s="25"/>
       <c r="G46" s="26"/>
@@ -2446,12 +2461,12 @@
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="51"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="37"/>
       <c r="E47" s="12"/>
       <c r="F47" s="27"/>
       <c r="G47" s="28"/>
@@ -2460,12 +2475,12 @@
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="68" t="s">
+      <c r="A48" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="69"/>
-      <c r="C48" s="69"/>
-      <c r="D48" s="70"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="49"/>
       <c r="E48" s="14">
         <f>SUM(E26:E47)</f>
         <v>0</v>
@@ -2478,25 +2493,25 @@
       <c r="H48" s="23"/>
     </row>
     <row r="49" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="55" t="s">
+      <c r="A49" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="56"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="64"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="56"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="49" t="s">
+      <c r="A50" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="50"/>
-      <c r="C50" s="50"/>
-      <c r="D50" s="51"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="37"/>
       <c r="E50" s="12">
         <v>5</v>
       </c>
@@ -2505,12 +2520,12 @@
       <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="51"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="37"/>
       <c r="E51" s="12">
         <v>5</v>
       </c>
@@ -2519,12 +2534,12 @@
       <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="51"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="37"/>
       <c r="E52" s="12">
         <v>5</v>
       </c>
@@ -2533,12 +2548,12 @@
       <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="49" t="s">
+      <c r="A53" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="50"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="51"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="37"/>
       <c r="E53" s="12">
         <v>10</v>
       </c>
@@ -2547,12 +2562,12 @@
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="49" t="s">
+      <c r="A54" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="50"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="51"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="37"/>
       <c r="E54" s="12">
         <v>50</v>
       </c>
@@ -2561,12 +2576,12 @@
       <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="49" t="s">
+      <c r="A55" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="51"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="37"/>
       <c r="E55" s="12">
         <v>10</v>
       </c>
@@ -2575,12 +2590,12 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="50"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="51"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="37"/>
       <c r="E56" s="12">
         <v>10</v>
       </c>
@@ -2589,12 +2604,12 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="49" t="s">
+      <c r="A57" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="51"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="37"/>
       <c r="E57" s="12">
         <v>20</v>
       </c>
@@ -2603,12 +2618,12 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="49" t="s">
+      <c r="A58" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="50"/>
-      <c r="C58" s="50"/>
-      <c r="D58" s="51"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="37"/>
       <c r="E58" s="12">
         <v>20</v>
       </c>
@@ -2617,12 +2632,12 @@
       <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="49" t="s">
+      <c r="A59" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="51"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="37"/>
       <c r="E59" s="12">
         <v>20</v>
       </c>
@@ -2631,12 +2646,12 @@
       <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="49" t="s">
+      <c r="A60" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="50"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="51"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="37"/>
       <c r="E60" s="12">
         <v>30</v>
       </c>
@@ -2645,12 +2660,12 @@
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="49" t="s">
+      <c r="A61" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="50"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="51"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="12">
         <v>10</v>
       </c>
@@ -2659,12 +2674,12 @@
       <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="49" t="s">
+      <c r="A62" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="50"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="51"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="12">
         <v>20</v>
       </c>
@@ -2673,12 +2688,12 @@
       <c r="H62" s="13"/>
     </row>
     <row r="63" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="49" t="s">
+      <c r="A63" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="50"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="51"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="37"/>
       <c r="E63" s="12">
         <v>30</v>
       </c>
@@ -2687,12 +2702,12 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="49" t="s">
+      <c r="A64" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="50"/>
-      <c r="C64" s="50"/>
-      <c r="D64" s="51"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="37"/>
       <c r="E64" s="12">
         <v>20</v>
       </c>
@@ -2701,12 +2716,12 @@
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="49" t="s">
+      <c r="A65" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="50"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="51"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="37"/>
       <c r="E65" s="12">
         <v>20</v>
       </c>
@@ -2715,12 +2730,12 @@
       <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="49" t="s">
+      <c r="A66" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="50"/>
-      <c r="C66" s="50"/>
-      <c r="D66" s="51"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="37"/>
       <c r="E66" s="12">
         <v>20</v>
       </c>
@@ -2729,12 +2744,12 @@
       <c r="H66" s="13"/>
     </row>
     <row r="67" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="49" t="s">
+      <c r="A67" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="50"/>
-      <c r="C67" s="50"/>
-      <c r="D67" s="51"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="37"/>
       <c r="E67" s="12">
         <v>20</v>
       </c>
@@ -2743,12 +2758,12 @@
       <c r="H67" s="13"/>
     </row>
     <row r="68" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="49" t="s">
+      <c r="A68" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="50"/>
-      <c r="C68" s="50"/>
-      <c r="D68" s="51"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="37"/>
       <c r="E68" s="24" t="s">
         <v>25</v>
       </c>
@@ -2759,12 +2774,12 @@
       <c r="H68" s="22"/>
     </row>
     <row r="69" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="52" t="s">
+      <c r="A69" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="53"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="54"/>
+      <c r="B69" s="45"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="46"/>
       <c r="E69" s="33">
         <f>SUM(E50:E67)</f>
         <v>325</v>
@@ -2777,12 +2792,12 @@
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="71" t="s">
+      <c r="A70" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B70" s="72"/>
-      <c r="C70" s="72"/>
-      <c r="D70" s="73"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="43"/>
       <c r="E70" s="30">
         <f>SUM(E7,E13,E18,E23)</f>
         <v>140</v>
@@ -3369,6 +3384,72 @@
     <row r="153" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A61:D61"/>
     <mergeCell ref="E25:H25"/>
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="E34:H34"/>
@@ -3385,72 +3466,6 @@
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Game mechanics and *fingerquotes* tunneling detection.
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>IGME 309 Final Project Fall 2013 Grading Guide</t>
   </si>
@@ -286,6 +286,18 @@
   </si>
   <si>
     <t>all header files</t>
+  </si>
+  <si>
+    <t>BezierSurfaceController.h</t>
+  </si>
+  <si>
+    <t>here it is.</t>
+  </si>
+  <si>
+    <t>GameController-&gt;endGame()</t>
+  </si>
+  <si>
+    <t>GameController.cpp</t>
   </si>
 </sst>
 </file>
@@ -1235,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,7 +2076,9 @@
         <v>10</v>
       </c>
       <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
+      <c r="G16" s="13" t="s">
+        <v>82</v>
+      </c>
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -2152,7 +2166,9 @@
         <v>20</v>
       </c>
       <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
+      <c r="G22" s="13" t="s">
+        <v>87</v>
+      </c>
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2243,7 +2259,9 @@
       <c r="D29" s="37"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
-      <c r="G29" s="13"/>
+      <c r="G29" s="13" t="s">
+        <v>90</v>
+      </c>
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2283,7 +2301,9 @@
       <c r="D32" s="37"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
-      <c r="G32" s="13"/>
+      <c r="G32" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2455,7 +2475,9 @@
       <c r="D46" s="37"/>
       <c r="E46" s="24"/>
       <c r="F46" s="25"/>
-      <c r="G46" s="26"/>
+      <c r="G46" s="26" t="s">
+        <v>88</v>
+      </c>
       <c r="H46" s="22"/>
       <c r="I46" s="2"/>
       <c r="J46" s="3"/>

</xml_diff>

<commit_message>
Added Cat Bowling title to menu screen
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -294,13 +294,13 @@
     <t>Comments above parts of code taken from other sources can be found in various files in the project</t>
   </si>
   <si>
-    <t>glm used for math instead of Angel, dynamic fragment colors for polyhedrons</t>
-  </si>
-  <si>
     <t>Inheritance is used with specialized polyhedrons</t>
   </si>
   <si>
     <t>See all files in project</t>
+  </si>
+  <si>
+    <t>glm used for math instead of Angel, dynamic fragment colors for polyhedrons, rotation with quaternions is used for rotating the octahedron</t>
   </si>
 </sst>
 </file>
@@ -847,6 +847,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -859,24 +901,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -886,14 +910,23 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -902,70 +935,37 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1835,58 +1835,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="70" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="71" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73">
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44">
         <f>((F70/E70)*100)</f>
         <v>0</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="71" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1902,25 +1902,25 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="6">
         <v>10</v>
       </c>
@@ -1929,12 +1929,12 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="8">
         <f>SUM(E6:E6)</f>
         <v>10</v>
@@ -1947,24 +1947,24 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="12">
         <v>10</v>
       </c>
@@ -1975,12 +1975,12 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="12">
         <v>10</v>
       </c>
@@ -1991,12 +1991,12 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="12">
         <v>10</v>
       </c>
@@ -2007,12 +2007,12 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="12">
         <v>10</v>
       </c>
@@ -2023,12 +2023,12 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="8">
         <f>SUM(E9:E12)</f>
         <v>40</v>
@@ -2041,24 +2041,24 @@
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="37"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="12">
         <v>10</v>
       </c>
@@ -2067,12 +2067,12 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="37"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="12">
         <v>10</v>
       </c>
@@ -2081,12 +2081,12 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="12">
         <v>40</v>
       </c>
@@ -2097,12 +2097,12 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="46"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="8">
         <f>SUM(E15:E17)</f>
         <v>60</v>
@@ -2115,24 +2115,24 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
     </row>
     <row r="20" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="12">
         <v>5</v>
       </c>
@@ -2141,12 +2141,12 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="12">
         <v>5</v>
       </c>
@@ -2155,12 +2155,12 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="51"/>
       <c r="E22" s="12">
         <v>20</v>
       </c>
@@ -2171,12 +2171,12 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="46"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="8">
         <f>SUM(E20:E22)</f>
         <v>30</v>
@@ -2189,37 +2189,37 @@
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:9" ht="29.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
     </row>
     <row r="26" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="13" t="s">
@@ -2228,12 +2228,12 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="13" t="s">
@@ -2242,48 +2242,48 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
     </row>
     <row r="29" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="37"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="37"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="51"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="37"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="13" t="s">
@@ -2292,88 +2292,88 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="51"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="37"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="51"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
     </row>
     <row r="35" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="51"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="37"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="51"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="37"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="51"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="51"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="13" t="s">
@@ -2382,12 +2382,12 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="51"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="13" t="s">
@@ -2396,12 +2396,12 @@
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="37"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="51"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="13" t="s">
@@ -2410,12 +2410,12 @@
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="37"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="51"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="13" t="s">
@@ -2424,60 +2424,60 @@
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
     </row>
     <row r="43" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="37"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="51"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="37"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="51"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="37"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="51"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="13"/>
       <c r="H45" s="21"/>
     </row>
     <row r="46" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="37"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="51"/>
       <c r="E46" s="24"/>
       <c r="F46" s="25"/>
       <c r="G46" s="26"/>
@@ -2486,12 +2486,12 @@
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="37"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="51"/>
       <c r="E47" s="12"/>
       <c r="F47" s="27"/>
       <c r="G47" s="28"/>
@@ -2500,12 +2500,12 @@
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="47" t="s">
+      <c r="A48" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="49"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="70"/>
       <c r="E48" s="14">
         <f>SUM(E26:E47)</f>
         <v>0</v>
@@ -2518,25 +2518,25 @@
       <c r="H48" s="23"/>
     </row>
     <row r="49" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="53" t="s">
+      <c r="A49" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="54"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="56"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="64"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="37"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="51"/>
       <c r="E50" s="12">
         <v>5</v>
       </c>
@@ -2545,12 +2545,12 @@
       <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="37"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="51"/>
       <c r="E51" s="12">
         <v>5</v>
       </c>
@@ -2559,12 +2559,12 @@
       <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="37"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="51"/>
       <c r="E52" s="12">
         <v>5</v>
       </c>
@@ -2573,12 +2573,12 @@
       <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="37"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="51"/>
       <c r="E53" s="12">
         <v>10</v>
       </c>
@@ -2587,12 +2587,12 @@
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="35" t="s">
+      <c r="A54" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="37"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="51"/>
       <c r="E54" s="12">
         <v>50</v>
       </c>
@@ -2601,12 +2601,12 @@
       <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="37"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="51"/>
       <c r="E55" s="12">
         <v>10</v>
       </c>
@@ -2615,12 +2615,12 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="37"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="51"/>
       <c r="E56" s="12">
         <v>10</v>
       </c>
@@ -2629,12 +2629,12 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="37"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="51"/>
       <c r="E57" s="12">
         <v>20</v>
       </c>
@@ -2643,12 +2643,12 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="37"/>
+      <c r="B58" s="50"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="51"/>
       <c r="E58" s="12">
         <v>20</v>
       </c>
@@ -2657,12 +2657,12 @@
       <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="35" t="s">
+      <c r="A59" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="37"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="51"/>
       <c r="E59" s="12">
         <v>20</v>
       </c>
@@ -2671,12 +2671,12 @@
       <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="37"/>
+      <c r="B60" s="50"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="51"/>
       <c r="E60" s="12">
         <v>30</v>
       </c>
@@ -2685,12 +2685,12 @@
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="37"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="51"/>
       <c r="E61" s="12">
         <v>10</v>
       </c>
@@ -2699,12 +2699,12 @@
       <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="35" t="s">
+      <c r="A62" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="37"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="51"/>
       <c r="E62" s="12">
         <v>20</v>
       </c>
@@ -2713,12 +2713,12 @@
       <c r="H62" s="13"/>
     </row>
     <row r="63" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="37"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="51"/>
       <c r="E63" s="12">
         <v>30</v>
       </c>
@@ -2727,12 +2727,12 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="37"/>
+      <c r="B64" s="50"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="51"/>
       <c r="E64" s="12">
         <v>20</v>
       </c>
@@ -2741,12 +2741,12 @@
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="35" t="s">
+      <c r="A65" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="37"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="51"/>
       <c r="E65" s="12">
         <v>20</v>
       </c>
@@ -2755,12 +2755,12 @@
       <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="37"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="51"/>
       <c r="E66" s="12">
         <v>20</v>
       </c>
@@ -2769,12 +2769,12 @@
       <c r="H66" s="13"/>
     </row>
     <row r="67" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="37"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="51"/>
       <c r="E67" s="12">
         <v>20</v>
       </c>
@@ -2783,28 +2783,28 @@
       <c r="H67" s="13"/>
     </row>
     <row r="68" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="35" t="s">
+      <c r="A68" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="37"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="51"/>
       <c r="E68" s="24" t="s">
         <v>25</v>
       </c>
       <c r="F68" s="29"/>
       <c r="G68" s="22" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H68" s="22"/>
     </row>
     <row r="69" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="44" t="s">
+      <c r="A69" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="46"/>
+      <c r="B69" s="53"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="54"/>
       <c r="E69" s="33">
         <f>SUM(E50:E67)</f>
         <v>325</v>
@@ -2817,12 +2817,12 @@
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B70" s="42"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="43"/>
+      <c r="B70" s="72"/>
+      <c r="C70" s="72"/>
+      <c r="D70" s="73"/>
       <c r="E70" s="30">
         <f>SUM(E7,E13,E18,E23)</f>
         <v>140</v>
@@ -3409,35 +3409,43 @@
     <row r="153" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A48:D48"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="E24:H24"/>
     <mergeCell ref="A64:D64"/>
@@ -3454,43 +3462,35 @@
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="A55:D55"/>
     <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added sound loops and sound effects to game
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="106">
   <si>
     <t>IGME 309 Final Project Fall 2013 Grading Guide</t>
   </si>
@@ -325,6 +325,24 @@
   </si>
   <si>
     <t>glm used for math instead of Angel, dynamic fragment colors for polyhedrons, rotation with quaternions is used for rotating the octahedron, made CB letters in the menu scene with polyhedrons.</t>
+  </si>
+  <si>
+    <t>AABB.h</t>
+  </si>
+  <si>
+    <t>Cleaned</t>
+  </si>
+  <si>
+    <t>Zipped.</t>
+  </si>
+  <si>
+    <t>Here it is.</t>
+  </si>
+  <si>
+    <t>See GameController.cpp-&gt;start()</t>
+  </si>
+  <si>
+    <t>See AABB.cpp-&gt;collisionResponseVector(Collider* other, glm::vec3 velocity) and GameController.cpp-&gt;update()</t>
   </si>
 </sst>
 </file>
@@ -871,6 +889,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -883,24 +943,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -910,14 +952,23 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -926,70 +977,37 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1275,7 +1293,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,58 +1877,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="70" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="71" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73">
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44">
         <f>((F70/E70)*100)</f>
         <v>0</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="71" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1926,25 +1944,25 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="6">
         <v>10</v>
       </c>
@@ -1955,12 +1973,12 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="8">
         <f>SUM(E6:E6)</f>
         <v>10</v>
@@ -1973,24 +1991,24 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="12">
         <v>10</v>
       </c>
@@ -2001,12 +2019,12 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="12">
         <v>10</v>
       </c>
@@ -2017,12 +2035,12 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="12">
         <v>10</v>
       </c>
@@ -2033,12 +2051,12 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="12">
         <v>10</v>
       </c>
@@ -2049,12 +2067,12 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="8">
         <f>SUM(E9:E12)</f>
         <v>40</v>
@@ -2067,52 +2085,56 @@
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="37"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="12">
         <v>10</v>
       </c>
       <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="37"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="12">
         <v>10</v>
       </c>
       <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
+      <c r="G16" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="12">
         <v>40</v>
       </c>
@@ -2123,12 +2145,12 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="46"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="8">
         <f>SUM(E15:E17)</f>
         <v>60</v>
@@ -2141,24 +2163,24 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
     </row>
     <row r="20" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="12">
         <v>5</v>
       </c>
@@ -2169,12 +2191,12 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="12">
         <v>5</v>
       </c>
@@ -2185,12 +2207,12 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="51"/>
       <c r="E22" s="12">
         <v>20</v>
       </c>
@@ -2201,12 +2223,12 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="46"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="8">
         <f>SUM(E20:E22)</f>
         <v>30</v>
@@ -2219,37 +2241,37 @@
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:9" ht="29.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
     </row>
     <row r="26" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="13" t="s">
@@ -2258,12 +2280,12 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="13" t="s">
@@ -2272,24 +2294,24 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
     </row>
     <row r="29" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="37"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="13" t="s">
@@ -2298,12 +2320,12 @@
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="37"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="51"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="13" t="s">
@@ -2312,12 +2334,12 @@
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="37"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="13" t="s">
@@ -2326,12 +2348,12 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="51"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="13" t="s">
@@ -2340,12 +2362,12 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="37"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="51"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="13" t="s">
@@ -2354,24 +2376,24 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
     </row>
     <row r="35" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="51"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="13" t="s">
@@ -2380,12 +2402,12 @@
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="37"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="51"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="13" t="s">
@@ -2394,12 +2416,12 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="37"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="51"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="13" t="s">
@@ -2408,12 +2430,12 @@
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="51"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="13" t="s">
@@ -2422,12 +2444,12 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="51"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="13" t="s">
@@ -2436,12 +2458,12 @@
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="37"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="51"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="13" t="s">
@@ -2450,12 +2472,12 @@
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="37"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="51"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="13" t="s">
@@ -2464,74 +2486,80 @@
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
     </row>
     <row r="43" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="37"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="51"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
-      <c r="G43" s="13"/>
+      <c r="G43" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="37"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="51"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
-      <c r="G44" s="13"/>
+      <c r="G44" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="37"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="51"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="13"/>
       <c r="H45" s="21"/>
     </row>
     <row r="46" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="37"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="51"/>
       <c r="E46" s="24"/>
       <c r="F46" s="25"/>
-      <c r="G46" s="26"/>
+      <c r="G46" s="26" t="s">
+        <v>103</v>
+      </c>
       <c r="H46" s="22"/>
       <c r="I46" s="2"/>
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="37"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="51"/>
       <c r="E47" s="12"/>
       <c r="F47" s="27"/>
       <c r="G47" s="28" t="s">
@@ -2542,12 +2570,12 @@
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="47" t="s">
+      <c r="A48" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="49"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="70"/>
       <c r="E48" s="14">
         <f>SUM(E26:E47)</f>
         <v>0</v>
@@ -2560,53 +2588,57 @@
       <c r="H48" s="23"/>
     </row>
     <row r="49" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="53" t="s">
+      <c r="A49" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="54"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="56"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="64"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="37"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="51"/>
       <c r="E50" s="12">
         <v>5</v>
       </c>
       <c r="F50" s="12"/>
-      <c r="G50" s="13"/>
+      <c r="G50" s="13" t="s">
+        <v>105</v>
+      </c>
       <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="37"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="51"/>
       <c r="E51" s="12">
         <v>5</v>
       </c>
       <c r="F51" s="12"/>
-      <c r="G51" s="13"/>
+      <c r="G51" s="13" t="s">
+        <v>104</v>
+      </c>
       <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="37"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="51"/>
       <c r="E52" s="12">
         <v>5</v>
       </c>
@@ -2615,12 +2647,12 @@
       <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="37"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="51"/>
       <c r="E53" s="12">
         <v>10</v>
       </c>
@@ -2629,12 +2661,12 @@
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="35" t="s">
+      <c r="A54" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="37"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="51"/>
       <c r="E54" s="12">
         <v>50</v>
       </c>
@@ -2645,12 +2677,12 @@
       <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="37"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="51"/>
       <c r="E55" s="12">
         <v>10</v>
       </c>
@@ -2659,12 +2691,12 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="37"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="51"/>
       <c r="E56" s="12">
         <v>10</v>
       </c>
@@ -2673,12 +2705,12 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="37"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="51"/>
       <c r="E57" s="12">
         <v>20</v>
       </c>
@@ -2687,12 +2719,12 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="37"/>
+      <c r="B58" s="50"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="51"/>
       <c r="E58" s="12">
         <v>20</v>
       </c>
@@ -2701,12 +2733,12 @@
       <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="35" t="s">
+      <c r="A59" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="37"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="51"/>
       <c r="E59" s="12">
         <v>20</v>
       </c>
@@ -2715,12 +2747,12 @@
       <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="37"/>
+      <c r="B60" s="50"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="51"/>
       <c r="E60" s="12">
         <v>30</v>
       </c>
@@ -2729,12 +2761,12 @@
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="37"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="51"/>
       <c r="E61" s="12">
         <v>10</v>
       </c>
@@ -2743,12 +2775,12 @@
       <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="35" t="s">
+      <c r="A62" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="37"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="51"/>
       <c r="E62" s="12">
         <v>20</v>
       </c>
@@ -2757,12 +2789,12 @@
       <c r="H62" s="13"/>
     </row>
     <row r="63" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="37"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="51"/>
       <c r="E63" s="12">
         <v>30</v>
       </c>
@@ -2771,12 +2803,12 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="37"/>
+      <c r="B64" s="50"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="51"/>
       <c r="E64" s="12">
         <v>20</v>
       </c>
@@ -2785,12 +2817,12 @@
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="35" t="s">
+      <c r="A65" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="37"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="51"/>
       <c r="E65" s="12">
         <v>20</v>
       </c>
@@ -2799,12 +2831,12 @@
       <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="37"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="51"/>
       <c r="E66" s="12">
         <v>20</v>
       </c>
@@ -2813,12 +2845,12 @@
       <c r="H66" s="13"/>
     </row>
     <row r="67" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="37"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="51"/>
       <c r="E67" s="12">
         <v>20</v>
       </c>
@@ -2827,12 +2859,12 @@
       <c r="H67" s="13"/>
     </row>
     <row r="68" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="35" t="s">
+      <c r="A68" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="37"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="51"/>
       <c r="E68" s="24" t="s">
         <v>25</v>
       </c>
@@ -2843,12 +2875,12 @@
       <c r="H68" s="22"/>
     </row>
     <row r="69" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="44" t="s">
+      <c r="A69" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="46"/>
+      <c r="B69" s="53"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="54"/>
       <c r="E69" s="33">
         <f>SUM(E50:E67)</f>
         <v>325</v>
@@ -2861,12 +2893,12 @@
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B70" s="42"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="43"/>
+      <c r="B70" s="72"/>
+      <c r="C70" s="72"/>
+      <c r="D70" s="73"/>
       <c r="E70" s="30">
         <f>SUM(E7,E13,E18,E23)</f>
         <v>140</v>
@@ -3453,35 +3485,43 @@
     <row r="153" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A48:D48"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="E24:H24"/>
     <mergeCell ref="A64:D64"/>
@@ -3498,43 +3538,35 @@
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="A55:D55"/>
     <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>